<commit_message>
Doing data analysis for NaNs
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
     <sheet name="browseNotes" sheetId="6" r:id="rId2"/>
     <sheet name="RejectStats" sheetId="7" r:id="rId3"/>
+    <sheet name="NaN Analysis" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="317">
   <si>
     <t>id</t>
   </si>
@@ -939,6 +940,45 @@
   </si>
   <si>
     <t>Standardize</t>
+  </si>
+  <si>
+    <t>verification_status</t>
+  </si>
+  <si>
+    <t>verification_status_joint</t>
+  </si>
+  <si>
+    <t>total_rev_hi_lim</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>NaNs</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>% Of Observations</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Remove? Don't know how to fill in values for NaNs</t>
+  </si>
+  <si>
+    <t>Fill in 0</t>
+  </si>
+  <si>
+    <t>Fill in 0?</t>
+  </si>
+  <si>
+    <t>Filter out these observations</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1354,8 +1394,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1518,8 +1564,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1608,8 +1761,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1690,8 +1851,62 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="6" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="13" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="4" borderId="13" xfId="8" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="13" xfId="6" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="6" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="19" xfId="6" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="96">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1743,6 +1958,10 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1771,6 +1990,10 @@
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2078,9 +2301,9 @@
   </sheetPr>
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2364,7 +2587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="45" customFormat="1">
+    <row r="26" spans="1:3" s="45" customFormat="1" ht="28">
       <c r="A26" s="43" t="s">
         <v>22</v>
       </c>
@@ -4240,4 +4463,916 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" style="58" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15" thickBot="1">
+      <c r="B1" s="81"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="81"/>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="82" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2" s="84" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" s="85" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="28">
+      <c r="B3" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="70" t="str">
+        <f>VLOOKUP(B3,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The combined self-reported annual income provided by the co-borrowers during registration</v>
+      </c>
+      <c r="D3" s="74">
+        <v>252970</v>
+      </c>
+      <c r="E3" s="77">
+        <f>D3/252971</f>
+        <v>0.99999604697771682</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="42">
+      <c r="B4" s="59" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="70" t="str">
+        <f>VLOOKUP(B4,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>A ratio calculated using the co-borrowers' total monthly payments on the total debt obligations, excluding mortgages and the requested LC loan, divided by the co-borrowers' combined self-reported monthly income</v>
+      </c>
+      <c r="D4" s="74">
+        <v>252970</v>
+      </c>
+      <c r="E4" s="77">
+        <f t="shared" ref="E4:E47" si="0">D4/252971</f>
+        <v>0.99999604697771682</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="59" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="70" t="e">
+        <f>VLOOKUP(B5,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="74">
+        <v>252970</v>
+      </c>
+      <c r="E5" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99999604697771682</v>
+      </c>
+      <c r="F5" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="70" t="str">
+        <f>VLOOKUP(B6,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Ratio of total current balance to high credit/credit limit on all install acct</v>
+      </c>
+      <c r="D6" s="74">
+        <v>252845</v>
+      </c>
+      <c r="E6" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99950191919231846</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="59" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="70" t="str">
+        <f>VLOOKUP(B7,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Months since most recent installment accounts opened</v>
+      </c>
+      <c r="D7" s="74">
+        <v>252831</v>
+      </c>
+      <c r="E7" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99944657688035388</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="70" t="str">
+        <f>VLOOKUP(B8,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of open trades in last 6 months</v>
+      </c>
+      <c r="D8" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E8" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F8" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="59" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" s="70" t="str">
+        <f>VLOOKUP(B9,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of currently active installment trades</v>
+      </c>
+      <c r="D9" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E9" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="59" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="70" t="str">
+        <f>VLOOKUP(B10,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of installment accounts opened in past 12 months</v>
+      </c>
+      <c r="D10" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E10" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F10" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="59" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="70" t="str">
+        <f>VLOOKUP(B11,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of installment accounts opened in past 24 months</v>
+      </c>
+      <c r="D11" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E11" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F11" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="59" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="70" t="str">
+        <f>VLOOKUP(B12,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Total current balance of all installment accounts</v>
+      </c>
+      <c r="D12" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E12" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" s="70" t="str">
+        <f>VLOOKUP(B13,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of revolving trades opened in past 12 months</v>
+      </c>
+      <c r="D13" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E13" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="70" t="str">
+        <f>VLOOKUP(B14,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of revolving trades opened in past 24 months</v>
+      </c>
+      <c r="D14" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E14" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="59" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="70" t="str">
+        <f>VLOOKUP(B15,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Maximum current balance owed on all revolving accounts</v>
+      </c>
+      <c r="D15" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E15" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="C16" s="70" t="str">
+        <f>VLOOKUP(B16,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Balance to credit limit on all trades</v>
+      </c>
+      <c r="D16" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E16" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="C17" s="70" t="str">
+        <f>VLOOKUP(B17,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of personal finance inquiries</v>
+      </c>
+      <c r="D17" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E17" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="59" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="70" t="str">
+        <f>VLOOKUP(B18,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of finance trades</v>
+      </c>
+      <c r="D18" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E18" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="59" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="70" t="str">
+        <f>VLOOKUP(B19,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of credit inquiries in past 12 months</v>
+      </c>
+      <c r="D19" s="74">
+        <v>252827</v>
+      </c>
+      <c r="E19" s="77">
+        <f t="shared" si="0"/>
+        <v>0.99943076479122117</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28">
+      <c r="B20" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="71" t="str">
+        <f>VLOOKUP(B20,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The number of months since the last public record.</v>
+      </c>
+      <c r="D20" s="75">
+        <v>221373</v>
+      </c>
+      <c r="E20" s="78">
+        <f t="shared" si="0"/>
+        <v>0.87509240189586945</v>
+      </c>
+      <c r="F20" s="62" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="28">
+      <c r="B21" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="71" t="str">
+        <f>VLOOKUP(B21,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The number of months since the borrower's last delinquency.</v>
+      </c>
+      <c r="D21" s="75">
+        <v>140820</v>
+      </c>
+      <c r="E21" s="78">
+        <f t="shared" si="0"/>
+        <v>0.55666459791833844</v>
+      </c>
+      <c r="F21" s="62" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="71" t="str">
+        <f>VLOOKUP(B22,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Total collection amounts ever owed</v>
+      </c>
+      <c r="D22" s="75">
+        <v>63708</v>
+      </c>
+      <c r="E22" s="78">
+        <f t="shared" si="0"/>
+        <v>0.25183914361725257</v>
+      </c>
+      <c r="F22" s="63" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="71" t="str">
+        <f>VLOOKUP(B23,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Total current balance of all accounts</v>
+      </c>
+      <c r="D23" s="75">
+        <v>63708</v>
+      </c>
+      <c r="E23" s="78">
+        <f t="shared" si="0"/>
+        <v>0.25183914361725257</v>
+      </c>
+      <c r="F23" s="63" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="C24" s="71" t="e">
+        <f>VLOOKUP(B24,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D24" s="75">
+        <v>63708</v>
+      </c>
+      <c r="E24" s="78">
+        <f t="shared" si="0"/>
+        <v>0.25183914361725257</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="28">
+      <c r="B25" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="72" t="str">
+        <f>VLOOKUP(B25,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v xml:space="preserve">Employment length in years. Possible values are between 0 and 10 where 0 means less than one year and 10 means ten or more years. </v>
+      </c>
+      <c r="D25" s="76">
+        <v>9897</v>
+      </c>
+      <c r="E25" s="79">
+        <f t="shared" si="0"/>
+        <v>3.9123061536697881E-2</v>
+      </c>
+      <c r="F25" s="65" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="28">
+      <c r="B26" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="72" t="str">
+        <f>VLOOKUP(B26,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Revolving line utilization rate, or the amount of credit the borrower is using relative to all available revolving credit.</v>
+      </c>
+      <c r="D26" s="76">
+        <v>199</v>
+      </c>
+      <c r="E26" s="79">
+        <f t="shared" si="0"/>
+        <v>7.8665143435413542E-4</v>
+      </c>
+      <c r="F26" s="65" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="72" t="str">
+        <f>VLOOKUP(B27,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>A unique LC assigned ID for the loan listing.</v>
+      </c>
+      <c r="D27" s="76">
+        <v>0</v>
+      </c>
+      <c r="E27" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="72" t="str">
+        <f>VLOOKUP(B28,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>A unique LC assigned Id for the borrower member.</v>
+      </c>
+      <c r="D28" s="76">
+        <v>0</v>
+      </c>
+      <c r="E28" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="28">
+      <c r="B29" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="72" t="str">
+        <f>VLOOKUP(B29,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The listed amount of the loan applied for by the borrower. If at some point in time, the credit department reduces the loan amount, then it will be reflected in this value.</v>
+      </c>
+      <c r="D29" s="76">
+        <v>0</v>
+      </c>
+      <c r="E29" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="72" t="str">
+        <f>VLOOKUP(B30,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The total amount committed to that loan at that point in time.</v>
+      </c>
+      <c r="D30" s="76">
+        <v>0</v>
+      </c>
+      <c r="E30" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="72" t="str">
+        <f>VLOOKUP(B31,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The total amount committed by investors for that loan at that point in time.</v>
+      </c>
+      <c r="D31" s="76">
+        <v>0</v>
+      </c>
+      <c r="E31" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="72" t="str">
+        <f>VLOOKUP(B32,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The monthly payment owed by the borrower if the loan originates.</v>
+      </c>
+      <c r="D32" s="76">
+        <v>0</v>
+      </c>
+      <c r="E32" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="28">
+      <c r="B33" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="72" t="str">
+        <f>VLOOKUP(B33,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The home ownership status provided by the borrower during registration. Our values are: RENT, OWN, MORTGAGE, OTHER.</v>
+      </c>
+      <c r="D33" s="76">
+        <v>0</v>
+      </c>
+      <c r="E33" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="72" t="str">
+        <f>VLOOKUP(B34,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The self-reported annual income provided by the borrower during registration.</v>
+      </c>
+      <c r="D34" s="76">
+        <v>0</v>
+      </c>
+      <c r="E34" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="64" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35" s="72" t="e">
+        <f>VLOOKUP(B35,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D35" s="76">
+        <v>0</v>
+      </c>
+      <c r="E35" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="72" t="str">
+        <f>VLOOKUP(B36,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v xml:space="preserve">A category provided by the borrower for the loan request. </v>
+      </c>
+      <c r="D36" s="76">
+        <v>0</v>
+      </c>
+      <c r="E36" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="72" t="str">
+        <f>VLOOKUP(B37,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The state provided by the borrower in the loan application</v>
+      </c>
+      <c r="D37" s="76">
+        <v>0</v>
+      </c>
+      <c r="E37" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="42">
+      <c r="B38" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="72" t="str">
+        <f>VLOOKUP(B38,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>A ratio calculated using the borrower’s total monthly debt payments on the total debt obligations, excluding mortgage and the requested LC loan, divided by the borrower’s self-reported monthly income.</v>
+      </c>
+      <c r="D38" s="76">
+        <v>0</v>
+      </c>
+      <c r="E38" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="28">
+      <c r="B39" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="72" t="str">
+        <f>VLOOKUP(B39,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The number of 30+ days past-due incidences of delinquency in the borrower's credit file for the past 2 years</v>
+      </c>
+      <c r="D39" s="76">
+        <v>0</v>
+      </c>
+      <c r="E39" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="72" t="str">
+        <f>VLOOKUP(B40,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The number of inquiries in past 6 months (excluding auto and mortgage inquiries)</v>
+      </c>
+      <c r="D40" s="76">
+        <v>0</v>
+      </c>
+      <c r="E40" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="72" t="str">
+        <f>VLOOKUP(B41,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The number of open credit lines in the borrower's credit file.</v>
+      </c>
+      <c r="D41" s="76">
+        <v>0</v>
+      </c>
+      <c r="E41" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="72" t="str">
+        <f>VLOOKUP(B42,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Number of derogatory public records</v>
+      </c>
+      <c r="D42" s="76">
+        <v>0</v>
+      </c>
+      <c r="E42" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="72" t="str">
+        <f>VLOOKUP(B43,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Total credit revolving balance</v>
+      </c>
+      <c r="D43" s="76">
+        <v>0</v>
+      </c>
+      <c r="E43" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="72" t="str">
+        <f>VLOOKUP(B44,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The total number of credit lines currently in the borrower's credit file</v>
+      </c>
+      <c r="D44" s="76">
+        <v>0</v>
+      </c>
+      <c r="E44" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="72" t="str">
+        <f>VLOOKUP(B45,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The initial listing status of the loan. Possible values are – W, F</v>
+      </c>
+      <c r="D45" s="76">
+        <v>0</v>
+      </c>
+      <c r="E45" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="28">
+      <c r="B46" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="C46" s="72" t="str">
+        <f>VLOOKUP(B46,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>Indicates whether the loan is an individual application or a joint application with two co-borrowers</v>
+      </c>
+      <c r="D46" s="76">
+        <v>0</v>
+      </c>
+      <c r="E46" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="15" thickBot="1">
+      <c r="B47" s="66" t="s">
+        <v>293</v>
+      </c>
+      <c r="C47" s="73" t="str">
+        <f>VLOOKUP(B47,LoanStats!$A$2:$B$80,2,FALSE)</f>
+        <v>The number of accounts on which the borrower is now delinquent.</v>
+      </c>
+      <c r="D47" s="86">
+        <v>0</v>
+      </c>
+      <c r="E47" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="67" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="C48" s="80"/>
+    </row>
+  </sheetData>
+  <sortState ref="B2:D46">
+    <sortCondition descending="1" ref="D2:D46"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>